<commit_message>
update slide_list path syntax
</commit_message>
<xml_diff>
--- a/test_files/slide_lists.xlsx
+++ b/test_files/slide_lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave2\Documents\PDX\PATHOverview-main\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EB2E48-9542-405D-87CF-6903D3736F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38EFBFB-8FB4-4337-B4B8-C9CFE36FDC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13260" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3870" yWindow="-14760" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slides" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Slide1</t>
   </si>
   <si>
-    <t>.\test_files</t>
-  </si>
-  <si>
     <t>OS-1.ndpi</t>
   </si>
   <si>
@@ -65,18 +62,12 @@
     <t>OS-2.ndpi</t>
   </si>
   <si>
-    <t>Slide1Sub</t>
-  </si>
-  <si>
     <t>(0.872831270292208, 0.2538111302759737)</t>
   </si>
   <si>
     <t>((0.8509156858766236, 0.25746372767857123), 0.42857142857142844, 0.4212662337662339)</t>
   </si>
   <si>
-    <t>Slide2Sub</t>
-  </si>
-  <si>
     <t>(0.7413377637987015, 0.5046228185876621)</t>
   </si>
   <si>
@@ -101,16 +92,25 @@
     <t>Page 1 Title</t>
   </si>
   <si>
-    <t>.\test_files\test_figure_output_1.tiff</t>
-  </si>
-  <si>
     <t>Page 2 Title</t>
   </si>
   <si>
     <t>Sub-views</t>
   </si>
   <si>
-    <t>.\test_files\test_figure_output_2.tiff</t>
+    <t>test_files\test_figure_output_1.tiff</t>
+  </si>
+  <si>
+    <t>test_files\test_figure_output_2.tiff</t>
+  </si>
+  <si>
+    <t>test_files</t>
+  </si>
+  <si>
+    <t>Slide1Crop</t>
+  </si>
+  <si>
+    <t>Slide2Crop</t>
   </si>
 </sst>
 </file>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -539,10 +539,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -553,16 +553,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -573,17 +573,17 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
       <c r="G4">
         <v>0</v>
       </c>
@@ -591,10 +591,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -605,16 +605,16 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -623,10 +623,10 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -652,19 +652,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -675,10 +675,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -689,13 +689,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>